<commit_message>
Made new dataset with the COVID data
</commit_message>
<xml_diff>
--- a/Data/COVIDData/ALLMONTHLYCOVIDDATA.xlsx
+++ b/Data/COVIDData/ALLMONTHLYCOVIDDATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\CodingProjectsStuff\2023SummerResearch-Inflation\COVID-Inflation\Data\COVIDData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9066AC-ED07-40FC-9120-89CA9DD29F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CC4824-4988-4C47-9713-0A2180508492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -364,9 +364,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A42" sqref="A41:A42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1002,35 +1004,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>45017</v>
-      </c>
-      <c r="B41">
-        <v>1195.5999999999999</v>
-      </c>
-      <c r="C41">
-        <v>47765.833333333336</v>
-      </c>
-      <c r="D41">
-        <v>13059.6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
-        <v>45047</v>
-      </c>
-      <c r="B42">
-        <v>531.66666666666663</v>
-      </c>
-      <c r="C42">
-        <v>69024.444444444438</v>
-      </c>
-      <c r="D42">
-        <v>9069.3333333333339</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
+      <c r="A41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Incorporated COVID data into the current models
</commit_message>
<xml_diff>
--- a/Data/COVIDData/ALLMONTHLYCOVIDDATA.xlsx
+++ b/Data/COVIDData/ALLMONTHLYCOVIDDATA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\CodingProjectsStuff\2023SummerResearch-Inflation\COVID-Inflation\Data\COVIDData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zs811\OneDrive\Documents\COVID-Inflation\Data\COVIDData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CC4824-4988-4C47-9713-0A2180508492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E6E4C0-A97F-47F2-8364-8E8FBDE83C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,16 +30,16 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Monthly Deaths</t>
-  </si>
-  <si>
-    <t>Monthly Vaccine Doses Admin</t>
-  </si>
-  <si>
     <t>Monthly Avg Hospital Admissions</t>
   </si>
   <si>
     <t>Monthly Avg Cases</t>
+  </si>
+  <si>
+    <t>Monthly Avg Vaccine Doses Admin</t>
+  </si>
+  <si>
+    <t>Monthly Avg Deaths</t>
   </si>
 </sst>
 </file>
@@ -366,35 +366,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A42" sqref="A41:A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43831</v>
       </c>
@@ -405,7 +405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43862</v>
       </c>
@@ -416,7 +416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43891</v>
       </c>
@@ -427,7 +427,7 @@
         <v>16838.75</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43922</v>
       </c>
@@ -438,7 +438,7 @@
         <v>194348.6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43952</v>
       </c>
@@ -449,7 +449,7 @@
         <v>163150.75</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43983</v>
       </c>
@@ -460,7 +460,7 @@
         <v>164665</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44013</v>
       </c>
@@ -471,7 +471,7 @@
         <v>399037.4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44044</v>
       </c>
@@ -485,7 +485,7 @@
         <v>363894.75</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44075</v>
       </c>
@@ -499,7 +499,7 @@
         <v>282161</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44105</v>
       </c>
@@ -513,7 +513,7 @@
         <v>405693</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44136</v>
       </c>
@@ -527,7 +527,7 @@
         <v>980243.75</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44166</v>
       </c>
@@ -544,7 +544,7 @@
         <v>1407933</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44197</v>
       </c>
@@ -561,7 +561,7 @@
         <v>1456146</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44228</v>
       </c>
@@ -578,7 +578,7 @@
         <v>665792.75</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44256</v>
       </c>
@@ -595,7 +595,7 @@
         <v>412179.8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44287</v>
       </c>
@@ -612,7 +612,7 @@
         <v>443665.75</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44317</v>
       </c>
@@ -629,7 +629,7 @@
         <v>243335.75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44348</v>
       </c>
@@ -646,7 +646,7 @@
         <v>98816.2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44378</v>
       </c>
@@ -663,7 +663,7 @@
         <v>286516.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44409</v>
       </c>
@@ -680,7 +680,7 @@
         <v>894632.5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44440</v>
       </c>
@@ -697,7 +697,7 @@
         <v>1001743.6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44470</v>
       </c>
@@ -714,7 +714,7 @@
         <v>587034.75</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44501</v>
       </c>
@@ -731,7 +731,7 @@
         <v>579798</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44531</v>
       </c>
@@ -748,7 +748,7 @@
         <v>1121519.3999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44562</v>
       </c>
@@ -765,7 +765,7 @@
         <v>4914461.25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44593</v>
       </c>
@@ -782,7 +782,7 @@
         <v>1410576.5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44621</v>
       </c>
@@ -799,7 +799,7 @@
         <v>246668.2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44652</v>
       </c>
@@ -816,7 +816,7 @@
         <v>272163.5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44682</v>
       </c>
@@ -833,7 +833,7 @@
         <v>632150</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44713</v>
       </c>
@@ -850,7 +850,7 @@
         <v>731743.2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44743</v>
       </c>
@@ -867,7 +867,7 @@
         <v>866428.75</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44774</v>
       </c>
@@ -884,7 +884,7 @@
         <v>712485.2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44805</v>
       </c>
@@ -901,7 +901,7 @@
         <v>432029.5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44835</v>
       </c>
@@ -918,7 +918,7 @@
         <v>275779.75</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44866</v>
       </c>
@@ -935,7 +935,7 @@
         <v>293323</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44896</v>
       </c>
@@ -952,7 +952,7 @@
         <v>456445.5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44927</v>
       </c>
@@ -969,7 +969,7 @@
         <v>389863</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44958</v>
       </c>
@@ -986,7 +986,7 @@
         <v>266807.25</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44986</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>175019.8</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Brent crude oil and new data, made LR and RF worse
</commit_message>
<xml_diff>
--- a/Data/COVIDData/ALLMONTHLYCOVIDDATA.xlsx
+++ b/Data/COVIDData/ALLMONTHLYCOVIDDATA.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zs811\OneDrive\Documents\COVID-Inflation\Data\COVIDData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\CodingProjectsStuff\2023SummerResearch-Inflation\COVID-Inflation\Data\COVIDData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E6E4C0-A97F-47F2-8364-8E8FBDE83C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0397F8-26BB-445A-8613-1656259C1B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -41,18 +52,32 @@
   <si>
     <t>Monthly Avg Deaths</t>
   </si>
+  <si>
+    <t>ChinaAvgCovidCases</t>
+  </si>
+  <si>
+    <t>ItalyAvgCovidCases</t>
+  </si>
+  <si>
+    <t>UKAvgCovidCases</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -63,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,11 +96,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -83,6 +123,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -364,20 +407,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="4" width="15" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" customWidth="1"/>
+    <col min="8" max="8" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -393,8 +439,17 @@
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43831</v>
       </c>
@@ -404,8 +459,17 @@
       <c r="E2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>335.17241379310337</v>
+      </c>
+      <c r="G2">
+        <v>0.125</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43862</v>
       </c>
@@ -415,8 +479,17 @@
       <c r="E3">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>2402.379310344827</v>
+      </c>
+      <c r="G3">
+        <v>30.517241379310349</v>
+      </c>
+      <c r="H3">
+        <v>1.931034482758621</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43891</v>
       </c>
@@ -426,8 +499,17 @@
       <c r="E4">
         <v>16838.75</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>101.8064516129032</v>
+      </c>
+      <c r="G4">
+        <v>3253.2580645161288</v>
+      </c>
+      <c r="H4">
+        <v>945.70967741935488</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>43922</v>
       </c>
@@ -437,8 +519,17 @@
       <c r="E5">
         <v>194348.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>60.93333333333333</v>
+      </c>
+      <c r="G5">
+        <v>3395.0666666666671</v>
+      </c>
+      <c r="H5">
+        <v>4567.3999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43952</v>
       </c>
@@ -448,8 +539,17 @@
       <c r="E6">
         <v>163150.75</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>6.354838709677419</v>
+      </c>
+      <c r="G6">
+        <v>937.83870967741939</v>
+      </c>
+      <c r="H6">
+        <v>2833.0645161290322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43983</v>
       </c>
@@ -459,8 +559,17 @@
       <c r="E7">
         <v>164665</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>21.9</v>
+      </c>
+      <c r="G7">
+        <v>272.36666666666667</v>
+      </c>
+      <c r="H7">
+        <v>973.33333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44013</v>
       </c>
@@ -470,8 +579,17 @@
       <c r="E8">
         <v>399037.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>88.032258064516128</v>
+      </c>
+      <c r="G8">
+        <v>216.83870967741939</v>
+      </c>
+      <c r="H8">
+        <v>665.9677419354839</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44044</v>
       </c>
@@ -484,8 +602,17 @@
       <c r="E9">
         <v>363894.75</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>78.290322580645167</v>
+      </c>
+      <c r="G9">
+        <v>679.35483870967744</v>
+      </c>
+      <c r="H9">
+        <v>1086.161290322581</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44075</v>
       </c>
@@ -498,8 +625,17 @@
       <c r="E10">
         <v>282161</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>21.93333333333333</v>
+      </c>
+      <c r="G10">
+        <v>1493.1</v>
+      </c>
+      <c r="H10">
+        <v>4366.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44105</v>
       </c>
@@ -512,8 +648,17 @@
       <c r="E11">
         <v>405693</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>27.483870967741939</v>
+      </c>
+      <c r="G11">
+        <v>10795.58064516129</v>
+      </c>
+      <c r="H11">
+        <v>18175.77419354839</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>44136</v>
       </c>
@@ -526,8 +671,17 @@
       <c r="E12">
         <v>980243.75</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>52.4</v>
+      </c>
+      <c r="G12">
+        <v>31250.133333333339</v>
+      </c>
+      <c r="H12">
+        <v>20629.633333333339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>44166</v>
       </c>
@@ -543,8 +697,17 @@
       <c r="E13">
         <v>1407933</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>103.48387096774189</v>
+      </c>
+      <c r="G13">
+        <v>16068.129032258061</v>
+      </c>
+      <c r="H13">
+        <v>29435.516129032261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>44197</v>
       </c>
@@ -560,8 +723,17 @@
       <c r="E14">
         <v>1456146</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>138.741935483871</v>
+      </c>
+      <c r="G14">
+        <v>14777.22580645161</v>
+      </c>
+      <c r="H14">
+        <v>42489.129032258068</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>44228</v>
       </c>
@@ -577,8 +749,17 @@
       <c r="E15">
         <v>665792.75</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>33.785714285714278</v>
+      </c>
+      <c r="G15">
+        <v>13072.928571428571</v>
+      </c>
+      <c r="H15">
+        <v>13091.642857142861</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>44256</v>
       </c>
@@ -594,8 +775,17 @@
       <c r="E16">
         <v>412179.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>27.161290322580641</v>
+      </c>
+      <c r="G16">
+        <v>21068.38709677419</v>
+      </c>
+      <c r="H16">
+        <v>5513.8709677419356</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>44287</v>
       </c>
@@ -611,8 +801,17 @@
       <c r="E17">
         <v>443665.75</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>28.666666666666671</v>
+      </c>
+      <c r="G17">
+        <v>14942.1</v>
+      </c>
+      <c r="H17">
+        <v>2651.333333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>44317</v>
       </c>
@@ -628,8 +827,17 @@
       <c r="E18">
         <v>243335.75</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>254.87096774193549</v>
+      </c>
+      <c r="G18">
+        <v>6670.8064516129034</v>
+      </c>
+      <c r="H18">
+        <v>2462.2258064516132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>44348</v>
       </c>
@@ -645,8 +853,17 @@
       <c r="E19">
         <v>98816.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>234.9666666666667</v>
+      </c>
+      <c r="G19">
+        <v>1437.666666666667</v>
+      </c>
+      <c r="H19">
+        <v>10617.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>44378</v>
       </c>
@@ -662,8 +879,17 @@
       <c r="E20">
         <v>286516.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>69.354838709677423</v>
+      </c>
+      <c r="G20">
+        <v>2722.1290322580639</v>
+      </c>
+      <c r="H20">
+        <v>34886.483870967742</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>44409</v>
       </c>
@@ -679,8 +905,17 @@
       <c r="E21">
         <v>894632.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>75.677419354838705</v>
+      </c>
+      <c r="G21">
+        <v>6160.6451612903229</v>
+      </c>
+      <c r="H21">
+        <v>30743.129032258061</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>44440</v>
       </c>
@@ -696,8 +931,17 @@
       <c r="E22">
         <v>1001743.6</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>53.5</v>
+      </c>
+      <c r="G22">
+        <v>4458.7333333333336</v>
+      </c>
+      <c r="H22">
+        <v>34492.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>44470</v>
       </c>
@@ -713,8 +957,17 @@
       <c r="E23">
         <v>587034.75</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>45.322580645161288</v>
+      </c>
+      <c r="G23">
+        <v>3199.322580645161</v>
+      </c>
+      <c r="H23">
+        <v>40996.548387096773</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>44501</v>
       </c>
@@ -730,8 +983,17 @@
       <c r="E24">
         <v>579798</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>62</v>
+      </c>
+      <c r="G24">
+        <v>8278.3333333333339</v>
+      </c>
+      <c r="H24">
+        <v>39566.133333333331</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>44531</v>
       </c>
@@ -747,8 +1009,17 @@
       <c r="E25">
         <v>1121519.3999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>133.32258064516131</v>
+      </c>
+      <c r="G25">
+        <v>31149.61290322581</v>
+      </c>
+      <c r="H25">
+        <v>97481.193548387091</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>44562</v>
       </c>
@@ -764,8 +1035,17 @@
       <c r="E26">
         <v>4914461.25</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>230.12903225806451</v>
+      </c>
+      <c r="G26">
+        <v>159485.70967741939</v>
+      </c>
+      <c r="H26">
+        <v>128591.6451612903</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>44593</v>
       </c>
@@ -781,8 +1061,17 @@
       <c r="E27">
         <v>1410576.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>7023.9642857142853</v>
+      </c>
+      <c r="G27">
+        <v>65681.178571428565</v>
+      </c>
+      <c r="H27">
+        <v>54571.357142857138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>44621</v>
       </c>
@@ -798,8 +1087,17 @@
       <c r="E28">
         <v>246668.2</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>18511.193548387098</v>
+      </c>
+      <c r="G28">
+        <v>58175.225806451614</v>
+      </c>
+      <c r="H28">
+        <v>70323.612903225803</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>44652</v>
       </c>
@@ -815,8 +1113,17 @@
       <c r="E29">
         <v>272163.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>6045.2333333333336</v>
+      </c>
+      <c r="G29">
+        <v>61373.1</v>
+      </c>
+      <c r="H29">
+        <v>30526.73333333333</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>44682</v>
       </c>
@@ -832,8 +1139,17 @@
       <c r="E30">
         <v>632150</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>62202.032258064522</v>
+      </c>
+      <c r="G30">
+        <v>31856.129032258061</v>
+      </c>
+      <c r="H30">
+        <v>8032.7419354838712</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>44713</v>
       </c>
@@ -849,8 +1165,17 @@
       <c r="E31">
         <v>731743.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>58334.133333333331</v>
+      </c>
+      <c r="G31">
+        <v>34738.466666666667</v>
+      </c>
+      <c r="H31">
+        <v>14085.73333333333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>44743</v>
       </c>
@@ -866,8 +1191,17 @@
       <c r="E32">
         <v>866428.75</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>27314.61290322581</v>
+      </c>
+      <c r="G32">
+        <v>82706.322580645166</v>
+      </c>
+      <c r="H32">
+        <v>19983.967741935481</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>44774</v>
       </c>
@@ -883,8 +1217,17 @@
       <c r="E33">
         <v>712485.2</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>25334</v>
+      </c>
+      <c r="G33">
+        <v>27199.032258064519</v>
+      </c>
+      <c r="H33">
+        <v>5762.2258064516127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>44805</v>
       </c>
@@ -900,8 +1243,17 @@
       <c r="E34">
         <v>432029.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>40566.73333333333</v>
+      </c>
+      <c r="G34">
+        <v>19562</v>
+      </c>
+      <c r="H34">
+        <v>5323.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>44835</v>
       </c>
@@ -917,8 +1269,17 @@
       <c r="E35">
         <v>275779.75</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>42870.93548387097</v>
+      </c>
+      <c r="G35">
+        <v>36023.225806451614</v>
+      </c>
+      <c r="H35">
+        <v>7665.322580645161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>44866</v>
       </c>
@@ -934,8 +1295,17 @@
       <c r="E36">
         <v>293323</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>23973.3</v>
+      </c>
+      <c r="G36">
+        <v>28832.76666666667</v>
+      </c>
+      <c r="H36">
+        <v>3464.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>44896</v>
       </c>
@@ -951,8 +1321,17 @@
       <c r="E37">
         <v>456445.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>2427689.2903225808</v>
+      </c>
+      <c r="G37">
+        <v>24320.38709677419</v>
+      </c>
+      <c r="H37">
+        <v>5538.0967741935483</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>44927</v>
       </c>
@@ -968,8 +1347,17 @@
       <c r="E38">
         <v>389863</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>437741.83870967739</v>
+      </c>
+      <c r="G38">
+        <v>9730.0645161290322</v>
+      </c>
+      <c r="H38">
+        <v>3035.1290322580639</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>44958</v>
       </c>
@@ -985,8 +1373,17 @@
       <c r="E39">
         <v>266807.25</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>19110.321428571431</v>
+      </c>
+      <c r="G39">
+        <v>4265.1071428571431</v>
+      </c>
+      <c r="H39">
+        <v>3631.821428571428</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>44986</v>
       </c>
@@ -1002,8 +1399,17 @@
       <c r="E40">
         <v>175019.8</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>6737.0967741935483</v>
+      </c>
+      <c r="G40">
+        <v>3413.483870967742</v>
+      </c>
+      <c r="H40">
+        <v>4341.6129032258068</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
     </row>
   </sheetData>

</xml_diff>